<commit_message>
update game 12 results
</commit_message>
<xml_diff>
--- a/boardgames/seafall/captains_log/glory.xlsx
+++ b/boardgames/seafall/captains_log/glory.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -700,7 +700,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -764,10 +763,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$C$2:$C$11</c:f>
+              <c:f>glory!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>11.0</c:v>
                 </c:pt>
@@ -797,6 +796,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -831,10 +836,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$D$2:$D$11</c:f>
+              <c:f>glory!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>6.0</c:v>
                 </c:pt>
@@ -864,6 +869,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,10 +909,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$E$2:$E$11</c:f>
+              <c:f>glory!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>6.0</c:v>
                 </c:pt>
@@ -931,6 +942,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -965,10 +982,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$F$2:$F$11</c:f>
+              <c:f>glory!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5.0</c:v>
                 </c:pt>
@@ -998,6 +1015,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1032,10 +1055,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$G$2:$G$11</c:f>
+              <c:f>glory!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -1065,6 +1088,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,11 +1109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-735001152"/>
-        <c:axId val="-873557504"/>
+        <c:axId val="1474486000"/>
+        <c:axId val="1349461904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-735001152"/>
+        <c:axId val="1474486000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1145,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1182,7 +1210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873557504"/>
+        <c:crossAx val="1349461904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1190,7 +1218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-873557504"/>
+        <c:axId val="1349461904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,7 +1264,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1297,7 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-735001152"/>
+        <c:crossAx val="1474486000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1311,7 +1338,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1418,7 +1444,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1798,11 +1823,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-735033952"/>
-        <c:axId val="-769535744"/>
+        <c:axId val="1347277840"/>
+        <c:axId val="1458577776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-735033952"/>
+        <c:axId val="1347277840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1839,7 +1864,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1905,7 +1929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-769535744"/>
+        <c:crossAx val="1458577776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1913,7 +1937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-769535744"/>
+        <c:axId val="1458577776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +1983,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2020,7 +2043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-735033952"/>
+        <c:crossAx val="1347277840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2034,7 +2057,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2146,7 +2168,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2210,10 +2231,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$M$2:$M$11</c:f>
+              <c:f>glory!$M$2:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -2243,6 +2264,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-22.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-23.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-24.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2277,10 +2304,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$N$2:$N$11</c:f>
+              <c:f>glory!$N$2:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>-5.0</c:v>
                 </c:pt>
@@ -2310,6 +2337,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-16.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-21.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2344,10 +2377,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$O$2:$O$11</c:f>
+              <c:f>glory!$O$2:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>-5.0</c:v>
                 </c:pt>
@@ -2377,6 +2410,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2411,10 +2450,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$P$2:$P$11</c:f>
+              <c:f>glory!$P$2:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>-6.0</c:v>
                 </c:pt>
@@ -2443,6 +2482,12 @@
                   <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2478,10 +2523,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>glory!$Q$2:$Q$11</c:f>
+              <c:f>glory!$Q$2:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>-7.0</c:v>
                 </c:pt>
@@ -2511,6 +2556,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>-13.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-18.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-19.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2526,11 +2577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-798134064"/>
-        <c:axId val="-798870240"/>
+        <c:axId val="1452298768"/>
+        <c:axId val="1452301312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-798134064"/>
+        <c:axId val="1452298768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2562,7 +2613,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2628,7 +2678,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-798870240"/>
+        <c:crossAx val="1452301312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2636,7 +2686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-798870240"/>
+        <c:axId val="1452301312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2687,7 +2737,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2748,7 +2797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-798134064"/>
+        <c:crossAx val="1452298768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2762,7 +2811,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2874,7 +2922,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2975,11 +3022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-765439856"/>
-        <c:axId val="-765176896"/>
+        <c:axId val="1452287888"/>
+        <c:axId val="1452290720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-765439856"/>
+        <c:axId val="1452287888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,7 +3068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-765176896"/>
+        <c:crossAx val="1452290720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3029,7 +3076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-765176896"/>
+        <c:axId val="1452290720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3080,7 +3127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-765439856"/>
+        <c:crossAx val="1452287888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5749,10 +5796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6976,48 +7023,155 @@
         <v>-18</v>
       </c>
       <c r="R12">
-        <f t="shared" ref="R12" si="20">RANK(C12,$C12:$G12)</f>
+        <f t="shared" ref="R12:R13" si="20">RANK(C12,$C12:$G12)</f>
         <v>3</v>
       </c>
       <c r="S12">
-        <f t="shared" ref="S12" si="21">RANK(D12,$C12:$G12)</f>
+        <f t="shared" ref="S12:S13" si="21">RANK(D12,$C12:$G12)</f>
         <v>4</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T12" si="22">RANK(E12,$C12:$G12)</f>
+        <f t="shared" ref="T12:T13" si="22">RANK(E12,$C12:$G12)</f>
         <v>1</v>
       </c>
       <c r="U12">
-        <f t="shared" ref="U12" si="23">RANK(F12,$C12:$G12)</f>
+        <f t="shared" ref="U12:U13" si="23">RANK(F12,$C12:$G12)</f>
         <v>2</v>
       </c>
       <c r="V12">
-        <f t="shared" ref="V12" si="24">RANK(G12,$C12:$G12)</f>
+        <f t="shared" ref="V12:V13" si="24">RANK(G12,$C12:$G12)</f>
         <v>4</v>
       </c>
       <c r="W12">
-        <f t="shared" ref="W12" si="25">C12/$B12</f>
+        <f t="shared" ref="W12:W13" si="25">C12/$B12</f>
         <v>0.61904761904761907</v>
       </c>
       <c r="X12">
-        <f t="shared" ref="X12" si="26">D12/$B12</f>
+        <f t="shared" ref="X12:X13" si="26">D12/$B12</f>
         <v>0.42857142857142855</v>
       </c>
       <c r="Y12">
-        <f t="shared" ref="Y12" si="27">E12/$B12</f>
+        <f t="shared" ref="Y12:Y13" si="27">E12/$B12</f>
         <v>1</v>
       </c>
       <c r="Z12">
-        <f t="shared" ref="Z12" si="28">F12/$B12</f>
+        <f t="shared" ref="Z12:Z13" si="28">F12/$B12</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AA12">
-        <f t="shared" ref="AA12" si="29">G12/$B12</f>
+        <f t="shared" ref="AA12:AA13" si="29">G12/$B12</f>
         <v>0.42857142857142855</v>
       </c>
       <c r="AB12">
-        <f t="shared" ref="AB12" si="30">SUM(C12:G12)</f>
+        <f t="shared" ref="AB12:AB13" si="30">SUM(C12:G12)</f>
         <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <f>SUM(C$2:C13)</f>
+        <v>123</v>
+      </c>
+      <c r="I13">
+        <f>SUM(D$2:D13)</f>
+        <v>135</v>
+      </c>
+      <c r="J13">
+        <f>SUM(E$2:E13)</f>
+        <v>145</v>
+      </c>
+      <c r="K13">
+        <f>SUM(F$2:F13)</f>
+        <v>147</v>
+      </c>
+      <c r="L13">
+        <f>SUM(G$2:G13)</f>
+        <v>128</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13" si="31">H13-MAX(H13:L13)</f>
+        <v>-24</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13" si="32">I13-MAX(H13:L13)</f>
+        <v>-12</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ref="O13" si="33">J13-MAX(H13:L13)</f>
+        <v>-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13" si="34">K13-MAX(H13:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ref="Q13" si="35">L13-MAX(H13:L13)</f>
+        <v>-19</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="23"/>
+        <v>3</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="24"/>
+        <v>4</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="25"/>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="26"/>
+        <v>1.1363636363636365</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="27"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="28"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="29"/>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="30"/>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>